<commit_message>
Commit After Chat Classification Prompt
</commit_message>
<xml_diff>
--- a/email_prompt_test/automation_testing_email.xlsx
+++ b/email_prompt_test/automation_testing_email.xlsx
@@ -1208,12 +1208,12 @@
       </c>
       <c r="E24" s="19" t="inlineStr">
         <is>
-          <t>PRODUCT_AVAILABILITY</t>
+          <t>OTHERS</t>
         </is>
       </c>
       <c r="F24" s="14" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="G24" s="25" t="n"/>
@@ -1368,12 +1368,12 @@
       </c>
       <c r="E29" s="19" t="inlineStr">
         <is>
-          <t>PRODUCT_AVAILABILITY</t>
+          <t>OTHERS</t>
         </is>
       </c>
       <c r="F29" s="14" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="G29" s="25" t="n"/>
@@ -2021,12 +2021,12 @@
       </c>
       <c r="E49" s="19" t="inlineStr">
         <is>
-          <t>BANTER</t>
+          <t>OTHERS</t>
         </is>
       </c>
       <c r="F49" s="14" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
     </row>
@@ -2409,12 +2409,12 @@
       </c>
       <c r="E61" s="26" t="inlineStr">
         <is>
-          <t>DAMAGES</t>
+          <t>OTHERS</t>
         </is>
       </c>
       <c r="F61" s="14" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
     </row>
@@ -2597,12 +2597,12 @@
       </c>
       <c r="E67" s="27" t="inlineStr">
         <is>
-          <t>PRODUCT_AVAILABILITY</t>
+          <t>OTHERS</t>
         </is>
       </c>
       <c r="F67" s="14" t="inlineStr">
         <is>
-          <t>PASS</t>
+          <t>FAIL</t>
         </is>
       </c>
     </row>
@@ -3076,12 +3076,12 @@
       </c>
       <c r="E82" s="27" t="inlineStr">
         <is>
-          <t>OTHERS</t>
+          <t>ORDER_STATUS</t>
         </is>
       </c>
       <c r="F82" s="14" t="inlineStr">
         <is>
-          <t>PASS</t>
+          <t>FAIL</t>
         </is>
       </c>
     </row>
@@ -3363,12 +3363,12 @@
       </c>
       <c r="E91" s="27" t="inlineStr">
         <is>
-          <t>BANTER</t>
+          <t>OTHERS</t>
         </is>
       </c>
       <c r="F91" s="14" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
     </row>
@@ -3769,12 +3769,12 @@
       </c>
       <c r="E104" s="27" t="inlineStr">
         <is>
-          <t>BANTER</t>
+          <t>OTHERS</t>
         </is>
       </c>
       <c r="F104" s="14" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
     </row>
@@ -4896,12 +4896,12 @@
       </c>
       <c r="E139" s="14" t="inlineStr">
         <is>
-          <t>ORDER_STATUS</t>
+          <t>OTHERS</t>
         </is>
       </c>
       <c r="F139" s="14" t="inlineStr">
         <is>
-          <t>PASS</t>
+          <t>FAIL</t>
         </is>
       </c>
     </row>

</xml_diff>